<commit_message>
getting close to final - now final data and code here
</commit_message>
<xml_diff>
--- a/data/book_tgt_climate_9.xlsx
+++ b/data/book_tgt_climate_9.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bill/Documents/R Projects/Project_Eddie/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72C68F6C-CC33-214B-ABE5-0EF619674624}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D243B365-B34C-B547-9C66-BD8337254330}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34280" yWindow="1360" windowWidth="20160" windowHeight="18020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34280" yWindow="1360" windowWidth="25840" windowHeight="18020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Temp (C)" sheetId="1" r:id="rId1"/>
@@ -82,12 +82,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Year</t>
   </si>
   <si>
     <t>Temperature</t>
+  </si>
+  <si>
+    <t># data from http://www.earth-policy.org/index.php?/data_center/C23/</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># downloaded 2019 - 06 -10 </t>
+  </si>
+  <si>
+    <t># added extra years at end</t>
   </si>
 </sst>
 </file>
@@ -1112,23 +1121,10 @@
     <xf numFmtId="0" fontId="60" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1138,15 +1134,19 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="170">
     <cellStyle name="20% - Accent1 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -1407,7 +1407,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Temp (C)'!$B$1</c:f>
+              <c:f>'Temp (C)'!$B$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1429,7 +1429,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Temp (C)'!$A$2:$A$136</c:f>
+              <c:f>'Temp (C)'!$A$5:$A$139</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="135"/>
@@ -1843,7 +1843,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Temp (C)'!$B$2:$B$136</c:f>
+              <c:f>'Temp (C)'!$B$5:$B$139</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="135"/>
@@ -3154,1470 +3154,1487 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr published="0"/>
-  <dimension ref="A1:E140"/>
+  <dimension ref="A1:E143"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A118" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B141" sqref="B141"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
   <cols>
-    <col min="2" max="2" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="8.83203125" style="1"/>
+    <col min="1" max="1" width="8.83203125" style="12"/>
+    <col min="2" max="2" width="17.5" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.83203125" style="8"/>
+    <col min="4" max="5" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B4" s="7" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="16">
-      <c r="A2" s="3">
+    <row r="5" spans="1:5" ht="16">
+      <c r="A5" s="3">
         <v>1880</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B5" s="5">
         <v>13.79</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="3">
-        <v>1881</v>
-      </c>
-      <c r="B3" s="4">
-        <v>13.87</v>
-      </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="3">
-        <v>1882</v>
-      </c>
-      <c r="B4" s="4">
-        <v>13.84</v>
-      </c>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="3">
-        <v>1883</v>
-      </c>
-      <c r="B5" s="4">
-        <v>13.81</v>
-      </c>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="3">
-        <v>1884</v>
-      </c>
-      <c r="B6" s="4">
-        <v>13.73</v>
-      </c>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
+        <v>1881</v>
+      </c>
+      <c r="B6" s="5">
+        <v>13.87</v>
+      </c>
+      <c r="C6" s="10"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="3">
-        <v>1885</v>
-      </c>
-      <c r="B7" s="4">
-        <v>13.75</v>
-      </c>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
+        <v>1882</v>
+      </c>
+      <c r="B7" s="5">
+        <v>13.84</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="3">
-        <v>1886</v>
-      </c>
-      <c r="B8" s="4">
-        <v>13.76</v>
-      </c>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
+        <v>1883</v>
+      </c>
+      <c r="B8" s="5">
+        <v>13.81</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="3">
-        <v>1887</v>
-      </c>
-      <c r="B9" s="4">
-        <v>13.69</v>
-      </c>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
+        <v>1884</v>
+      </c>
+      <c r="B9" s="5">
+        <v>13.73</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="3">
-        <v>1888</v>
-      </c>
-      <c r="B10" s="4">
-        <v>13.81</v>
-      </c>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
+        <v>1885</v>
+      </c>
+      <c r="B10" s="5">
+        <v>13.75</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="3">
-        <v>1889</v>
-      </c>
-      <c r="B11" s="4">
-        <v>13.9</v>
-      </c>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
+        <v>1886</v>
+      </c>
+      <c r="B11" s="5">
+        <v>13.76</v>
+      </c>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="3">
-        <v>1890</v>
-      </c>
-      <c r="B12" s="4">
-        <v>13.67</v>
-      </c>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
+        <v>1887</v>
+      </c>
+      <c r="B12" s="5">
+        <v>13.69</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="3">
-        <v>1891</v>
-      </c>
-      <c r="B13" s="4">
-        <v>13.73</v>
-      </c>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
+        <v>1888</v>
+      </c>
+      <c r="B13" s="5">
+        <v>13.81</v>
+      </c>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="3">
-        <v>1892</v>
-      </c>
-      <c r="B14" s="4">
-        <v>13.69</v>
-      </c>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
+        <v>1889</v>
+      </c>
+      <c r="B14" s="5">
+        <v>13.9</v>
+      </c>
+      <c r="C14" s="11"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="3">
-        <v>1893</v>
-      </c>
-      <c r="B15" s="4">
-        <v>13.64</v>
-      </c>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
+        <v>1890</v>
+      </c>
+      <c r="B15" s="5">
+        <v>13.67</v>
+      </c>
+      <c r="C15" s="11"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="3">
-        <v>1894</v>
-      </c>
-      <c r="B16" s="4">
-        <v>13.68</v>
-      </c>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
+        <v>1891</v>
+      </c>
+      <c r="B16" s="5">
+        <v>13.73</v>
+      </c>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="3">
-        <v>1895</v>
-      </c>
-      <c r="B17" s="4">
-        <v>13.75</v>
-      </c>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
+        <v>1892</v>
+      </c>
+      <c r="B17" s="5">
+        <v>13.69</v>
+      </c>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="3">
-        <v>1896</v>
-      </c>
-      <c r="B18" s="4">
-        <v>13.83</v>
-      </c>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
+        <v>1893</v>
+      </c>
+      <c r="B18" s="5">
+        <v>13.64</v>
+      </c>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="3">
-        <v>1897</v>
-      </c>
-      <c r="B19" s="4">
-        <v>13.82</v>
-      </c>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
+        <v>1894</v>
+      </c>
+      <c r="B19" s="5">
+        <v>13.68</v>
+      </c>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="3">
-        <v>1898</v>
-      </c>
-      <c r="B20" s="4">
-        <v>13.69</v>
-      </c>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
+        <v>1895</v>
+      </c>
+      <c r="B20" s="5">
+        <v>13.75</v>
+      </c>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="3">
-        <v>1899</v>
-      </c>
-      <c r="B21" s="4">
-        <v>13.8</v>
-      </c>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
+        <v>1896</v>
+      </c>
+      <c r="B21" s="5">
+        <v>13.83</v>
+      </c>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="3">
-        <v>1900</v>
-      </c>
-      <c r="B22" s="4">
-        <v>13.85</v>
-      </c>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
+        <v>1897</v>
+      </c>
+      <c r="B22" s="5">
+        <v>13.82</v>
+      </c>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="3">
-        <v>1901</v>
-      </c>
-      <c r="B23" s="4">
-        <v>13.79</v>
-      </c>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
+        <v>1898</v>
+      </c>
+      <c r="B23" s="5">
+        <v>13.69</v>
+      </c>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="3">
-        <v>1902</v>
-      </c>
-      <c r="B24" s="4">
-        <v>13.7</v>
-      </c>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
+        <v>1899</v>
+      </c>
+      <c r="B24" s="5">
+        <v>13.8</v>
+      </c>
+      <c r="C24" s="11"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="3">
-        <v>1903</v>
-      </c>
-      <c r="B25" s="4">
-        <v>13.64</v>
-      </c>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
+        <v>1900</v>
+      </c>
+      <c r="B25" s="5">
+        <v>13.85</v>
+      </c>
+      <c r="C25" s="11"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="3">
-        <v>1904</v>
-      </c>
-      <c r="B26" s="4">
-        <v>13.56</v>
-      </c>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
+        <v>1901</v>
+      </c>
+      <c r="B26" s="5">
+        <v>13.79</v>
+      </c>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="3">
-        <v>1905</v>
-      </c>
-      <c r="B27" s="4">
-        <v>13.71</v>
-      </c>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
+        <v>1902</v>
+      </c>
+      <c r="B27" s="5">
+        <v>13.7</v>
+      </c>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="3">
-        <v>1906</v>
-      </c>
-      <c r="B28" s="4">
-        <v>13.74</v>
-      </c>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
+        <v>1903</v>
+      </c>
+      <c r="B28" s="5">
+        <v>13.64</v>
+      </c>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="3">
-        <v>1907</v>
-      </c>
-      <c r="B29" s="4">
-        <v>13.58</v>
-      </c>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
+        <v>1904</v>
+      </c>
+      <c r="B29" s="5">
+        <v>13.56</v>
+      </c>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="3">
-        <v>1908</v>
-      </c>
-      <c r="B30" s="4">
-        <v>13.57</v>
-      </c>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
+        <v>1905</v>
+      </c>
+      <c r="B30" s="5">
+        <v>13.71</v>
+      </c>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="3">
-        <v>1909</v>
-      </c>
-      <c r="B31" s="4">
-        <v>13.53</v>
-      </c>
-      <c r="C31" s="6"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="6"/>
+        <v>1906</v>
+      </c>
+      <c r="B31" s="5">
+        <v>13.74</v>
+      </c>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="3">
-        <v>1910</v>
-      </c>
-      <c r="B32" s="4">
-        <v>13.54</v>
-      </c>
-      <c r="C32" s="6"/>
-      <c r="D32" s="6"/>
-      <c r="E32" s="6"/>
+        <v>1907</v>
+      </c>
+      <c r="B32" s="5">
+        <v>13.58</v>
+      </c>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="3">
-        <v>1911</v>
-      </c>
-      <c r="B33" s="4">
-        <v>13.56</v>
-      </c>
-      <c r="D33" s="6"/>
-      <c r="E33" s="6"/>
+        <v>1908</v>
+      </c>
+      <c r="B33" s="5">
+        <v>13.57</v>
+      </c>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="3">
-        <v>1912</v>
-      </c>
-      <c r="B34" s="4">
-        <v>13.59</v>
-      </c>
-      <c r="D34" s="6"/>
-      <c r="E34" s="6"/>
+        <v>1909</v>
+      </c>
+      <c r="B34" s="5">
+        <v>13.53</v>
+      </c>
+      <c r="C34" s="11"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="3">
-        <v>1913</v>
-      </c>
-      <c r="B35" s="4">
-        <v>13.61</v>
-      </c>
-      <c r="D35" s="6"/>
-      <c r="E35" s="6"/>
+        <v>1910</v>
+      </c>
+      <c r="B35" s="5">
+        <v>13.54</v>
+      </c>
+      <c r="C35" s="11"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="3">
-        <v>1914</v>
-      </c>
-      <c r="B36" s="4">
-        <v>13.78</v>
-      </c>
-      <c r="D36" s="6"/>
-      <c r="E36" s="6"/>
+        <v>1911</v>
+      </c>
+      <c r="B36" s="5">
+        <v>13.56</v>
+      </c>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="3">
-        <v>1915</v>
-      </c>
-      <c r="B37" s="4">
-        <v>13.84</v>
-      </c>
-      <c r="D37" s="6"/>
-      <c r="E37" s="6"/>
+        <v>1912</v>
+      </c>
+      <c r="B37" s="5">
+        <v>13.59</v>
+      </c>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="3">
-        <v>1916</v>
-      </c>
-      <c r="B38" s="4">
-        <v>13.65</v>
-      </c>
-      <c r="D38" s="6"/>
-      <c r="E38" s="6"/>
+        <v>1913</v>
+      </c>
+      <c r="B38" s="5">
+        <v>13.61</v>
+      </c>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="3">
-        <v>1917</v>
-      </c>
-      <c r="B39" s="4">
-        <v>13.57</v>
-      </c>
-      <c r="D39" s="6"/>
-      <c r="E39" s="6"/>
+        <v>1914</v>
+      </c>
+      <c r="B39" s="5">
+        <v>13.78</v>
+      </c>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="3">
-        <v>1918</v>
-      </c>
-      <c r="B40" s="4">
-        <v>13.69</v>
-      </c>
-      <c r="D40" s="6"/>
-      <c r="E40" s="6"/>
+        <v>1915</v>
+      </c>
+      <c r="B40" s="5">
+        <v>13.84</v>
+      </c>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="3">
-        <v>1919</v>
-      </c>
-      <c r="B41" s="4">
-        <v>13.71</v>
-      </c>
-      <c r="C41" s="6"/>
-      <c r="D41" s="6"/>
-      <c r="E41" s="6"/>
+        <v>1916</v>
+      </c>
+      <c r="B41" s="5">
+        <v>13.65</v>
+      </c>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="3">
-        <v>1920</v>
-      </c>
-      <c r="B42" s="4">
-        <v>13.73</v>
-      </c>
-      <c r="C42" s="6"/>
-      <c r="D42" s="6"/>
-      <c r="E42" s="6"/>
+        <v>1917</v>
+      </c>
+      <c r="B42" s="5">
+        <v>13.57</v>
+      </c>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="3">
-        <v>1921</v>
-      </c>
-      <c r="B43" s="4">
-        <v>13.8</v>
-      </c>
-      <c r="D43" s="6"/>
-      <c r="E43" s="6"/>
+        <v>1918</v>
+      </c>
+      <c r="B43" s="5">
+        <v>13.69</v>
+      </c>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="3">
-        <v>1922</v>
-      </c>
-      <c r="B44" s="4">
+        <v>1919</v>
+      </c>
+      <c r="B44" s="5">
         <v>13.71</v>
       </c>
-      <c r="D44" s="6"/>
-      <c r="E44" s="6"/>
+      <c r="C44" s="11"/>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="3">
-        <v>1923</v>
-      </c>
-      <c r="B45" s="4">
-        <v>13.75</v>
-      </c>
-      <c r="D45" s="6"/>
-      <c r="E45" s="6"/>
+        <v>1920</v>
+      </c>
+      <c r="B45" s="5">
+        <v>13.73</v>
+      </c>
+      <c r="C45" s="11"/>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="3">
-        <v>1924</v>
-      </c>
-      <c r="B46" s="4">
-        <v>13.76</v>
-      </c>
-      <c r="D46" s="6"/>
-      <c r="E46" s="6"/>
+        <v>1921</v>
+      </c>
+      <c r="B46" s="5">
+        <v>13.8</v>
+      </c>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="3">
-        <v>1925</v>
-      </c>
-      <c r="B47" s="4">
-        <v>13.79</v>
-      </c>
-      <c r="D47" s="6"/>
-      <c r="E47" s="6"/>
+        <v>1922</v>
+      </c>
+      <c r="B47" s="5">
+        <v>13.71</v>
+      </c>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2"/>
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="3">
-        <v>1926</v>
-      </c>
-      <c r="B48" s="4">
-        <v>13.91</v>
-      </c>
-      <c r="D48" s="6"/>
-      <c r="E48" s="6"/>
+        <v>1923</v>
+      </c>
+      <c r="B48" s="5">
+        <v>13.75</v>
+      </c>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2"/>
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="3">
-        <v>1927</v>
-      </c>
-      <c r="B49" s="4">
-        <v>13.82</v>
-      </c>
-      <c r="D49" s="6"/>
-      <c r="E49" s="6"/>
+        <v>1924</v>
+      </c>
+      <c r="B49" s="5">
+        <v>13.76</v>
+      </c>
+      <c r="D49" s="2"/>
+      <c r="E49" s="2"/>
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="3">
-        <v>1928</v>
-      </c>
-      <c r="B50" s="4">
-        <v>13.84</v>
-      </c>
-      <c r="D50" s="6"/>
-      <c r="E50" s="6"/>
+        <v>1925</v>
+      </c>
+      <c r="B50" s="5">
+        <v>13.79</v>
+      </c>
+      <c r="D50" s="2"/>
+      <c r="E50" s="2"/>
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="3">
-        <v>1929</v>
-      </c>
-      <c r="B51" s="4">
-        <v>13.69</v>
-      </c>
-      <c r="C51" s="6"/>
-      <c r="D51" s="6"/>
-      <c r="E51" s="6"/>
+        <v>1926</v>
+      </c>
+      <c r="B51" s="5">
+        <v>13.91</v>
+      </c>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2"/>
     </row>
     <row r="52" spans="1:5">
       <c r="A52" s="3">
-        <v>1930</v>
-      </c>
-      <c r="B52" s="4">
-        <v>13.88</v>
-      </c>
-      <c r="C52" s="6"/>
-      <c r="D52" s="6"/>
-      <c r="E52" s="6"/>
+        <v>1927</v>
+      </c>
+      <c r="B52" s="5">
+        <v>13.82</v>
+      </c>
+      <c r="D52" s="2"/>
+      <c r="E52" s="2"/>
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="3">
-        <v>1931</v>
-      </c>
-      <c r="B53" s="4">
-        <v>13.93</v>
-      </c>
-      <c r="D53" s="6"/>
-      <c r="E53" s="6"/>
+        <v>1928</v>
+      </c>
+      <c r="B53" s="5">
+        <v>13.84</v>
+      </c>
+      <c r="D53" s="2"/>
+      <c r="E53" s="2"/>
     </row>
     <row r="54" spans="1:5">
       <c r="A54" s="3">
-        <v>1932</v>
-      </c>
-      <c r="B54" s="4">
-        <v>13.89</v>
-      </c>
-      <c r="D54" s="6"/>
-      <c r="E54" s="6"/>
+        <v>1929</v>
+      </c>
+      <c r="B54" s="5">
+        <v>13.69</v>
+      </c>
+      <c r="C54" s="11"/>
+      <c r="D54" s="2"/>
+      <c r="E54" s="2"/>
     </row>
     <row r="55" spans="1:5">
       <c r="A55" s="3">
-        <v>1933</v>
-      </c>
-      <c r="B55" s="4">
-        <v>13.75</v>
-      </c>
-      <c r="D55" s="6"/>
-      <c r="E55" s="6"/>
+        <v>1930</v>
+      </c>
+      <c r="B55" s="5">
+        <v>13.88</v>
+      </c>
+      <c r="C55" s="11"/>
+      <c r="D55" s="2"/>
+      <c r="E55" s="2"/>
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="3">
-        <v>1934</v>
-      </c>
-      <c r="B56" s="4">
-        <v>13.91</v>
-      </c>
-      <c r="D56" s="6"/>
-      <c r="E56" s="6"/>
+        <v>1931</v>
+      </c>
+      <c r="B56" s="5">
+        <v>13.93</v>
+      </c>
+      <c r="D56" s="2"/>
+      <c r="E56" s="2"/>
     </row>
     <row r="57" spans="1:5">
       <c r="A57" s="3">
-        <v>1935</v>
-      </c>
-      <c r="B57" s="4">
-        <v>13.85</v>
-      </c>
-      <c r="D57" s="6"/>
-      <c r="E57" s="6"/>
+        <v>1932</v>
+      </c>
+      <c r="B57" s="5">
+        <v>13.89</v>
+      </c>
+      <c r="D57" s="2"/>
+      <c r="E57" s="2"/>
     </row>
     <row r="58" spans="1:5">
       <c r="A58" s="3">
-        <v>1936</v>
-      </c>
-      <c r="B58" s="4">
-        <v>13.9</v>
-      </c>
-      <c r="D58" s="6"/>
-      <c r="E58" s="6"/>
+        <v>1933</v>
+      </c>
+      <c r="B58" s="5">
+        <v>13.75</v>
+      </c>
+      <c r="D58" s="2"/>
+      <c r="E58" s="2"/>
     </row>
     <row r="59" spans="1:5">
       <c r="A59" s="3">
-        <v>1937</v>
-      </c>
-      <c r="B59" s="4">
-        <v>14.03</v>
-      </c>
-      <c r="D59" s="6"/>
-      <c r="E59" s="6"/>
+        <v>1934</v>
+      </c>
+      <c r="B59" s="5">
+        <v>13.91</v>
+      </c>
+      <c r="D59" s="2"/>
+      <c r="E59" s="2"/>
     </row>
     <row r="60" spans="1:5">
       <c r="A60" s="3">
-        <v>1938</v>
-      </c>
-      <c r="B60" s="4">
-        <v>14.06</v>
-      </c>
-      <c r="D60" s="6"/>
-      <c r="E60" s="6"/>
+        <v>1935</v>
+      </c>
+      <c r="B60" s="5">
+        <v>13.85</v>
+      </c>
+      <c r="D60" s="2"/>
+      <c r="E60" s="2"/>
     </row>
     <row r="61" spans="1:5">
       <c r="A61" s="3">
-        <v>1939</v>
-      </c>
-      <c r="B61" s="4">
-        <v>14.01</v>
-      </c>
-      <c r="C61" s="6"/>
-      <c r="D61" s="6"/>
-      <c r="E61" s="6"/>
+        <v>1936</v>
+      </c>
+      <c r="B61" s="5">
+        <v>13.9</v>
+      </c>
+      <c r="D61" s="2"/>
+      <c r="E61" s="2"/>
     </row>
     <row r="62" spans="1:5">
       <c r="A62" s="3">
-        <v>1940</v>
-      </c>
-      <c r="B62" s="4">
-        <v>14.07</v>
-      </c>
-      <c r="C62" s="6"/>
-      <c r="D62" s="6"/>
-      <c r="E62" s="6"/>
+        <v>1937</v>
+      </c>
+      <c r="B62" s="5">
+        <v>14.03</v>
+      </c>
+      <c r="D62" s="2"/>
+      <c r="E62" s="2"/>
     </row>
     <row r="63" spans="1:5">
       <c r="A63" s="3">
-        <v>1941</v>
-      </c>
-      <c r="B63" s="4">
-        <v>14.08</v>
-      </c>
-      <c r="D63" s="6"/>
-      <c r="E63" s="6"/>
+        <v>1938</v>
+      </c>
+      <c r="B63" s="5">
+        <v>14.06</v>
+      </c>
+      <c r="D63" s="2"/>
+      <c r="E63" s="2"/>
     </row>
     <row r="64" spans="1:5">
       <c r="A64" s="3">
-        <v>1942</v>
-      </c>
-      <c r="B64" s="4">
-        <v>14.05</v>
-      </c>
-      <c r="D64" s="6"/>
-      <c r="E64" s="6"/>
+        <v>1939</v>
+      </c>
+      <c r="B64" s="5">
+        <v>14.01</v>
+      </c>
+      <c r="C64" s="11"/>
+      <c r="D64" s="2"/>
+      <c r="E64" s="2"/>
     </row>
     <row r="65" spans="1:5">
       <c r="A65" s="3">
-        <v>1943</v>
-      </c>
-      <c r="B65" s="4">
-        <v>14.06</v>
-      </c>
-      <c r="D65" s="6"/>
-      <c r="E65" s="6"/>
+        <v>1940</v>
+      </c>
+      <c r="B65" s="5">
+        <v>14.07</v>
+      </c>
+      <c r="C65" s="11"/>
+      <c r="D65" s="2"/>
+      <c r="E65" s="2"/>
     </row>
     <row r="66" spans="1:5">
       <c r="A66" s="3">
-        <v>1944</v>
-      </c>
-      <c r="B66" s="4">
-        <v>14.14</v>
-      </c>
-      <c r="D66" s="6"/>
-      <c r="E66" s="6"/>
+        <v>1941</v>
+      </c>
+      <c r="B66" s="5">
+        <v>14.08</v>
+      </c>
+      <c r="D66" s="2"/>
+      <c r="E66" s="2"/>
     </row>
     <row r="67" spans="1:5">
       <c r="A67" s="3">
-        <v>1945</v>
-      </c>
-      <c r="B67" s="4">
-        <v>14.01</v>
-      </c>
-      <c r="D67" s="6"/>
-      <c r="E67" s="6"/>
+        <v>1942</v>
+      </c>
+      <c r="B67" s="5">
+        <v>14.05</v>
+      </c>
+      <c r="D67" s="2"/>
+      <c r="E67" s="2"/>
     </row>
     <row r="68" spans="1:5">
       <c r="A68" s="3">
-        <v>1946</v>
-      </c>
-      <c r="B68" s="4">
-        <v>13.93</v>
-      </c>
-      <c r="D68" s="6"/>
-      <c r="E68" s="6"/>
+        <v>1943</v>
+      </c>
+      <c r="B68" s="5">
+        <v>14.06</v>
+      </c>
+      <c r="D68" s="2"/>
+      <c r="E68" s="2"/>
     </row>
     <row r="69" spans="1:5">
       <c r="A69" s="3">
-        <v>1947</v>
-      </c>
-      <c r="B69" s="4">
-        <v>13.96</v>
-      </c>
-      <c r="D69" s="6"/>
-      <c r="E69" s="6"/>
+        <v>1944</v>
+      </c>
+      <c r="B69" s="5">
+        <v>14.14</v>
+      </c>
+      <c r="D69" s="2"/>
+      <c r="E69" s="2"/>
     </row>
     <row r="70" spans="1:5">
       <c r="A70" s="3">
-        <v>1948</v>
-      </c>
-      <c r="B70" s="4">
-        <v>13.9</v>
-      </c>
-      <c r="D70" s="6"/>
-      <c r="E70" s="6"/>
+        <v>1945</v>
+      </c>
+      <c r="B70" s="5">
+        <v>14.01</v>
+      </c>
+      <c r="D70" s="2"/>
+      <c r="E70" s="2"/>
     </row>
     <row r="71" spans="1:5">
       <c r="A71" s="3">
-        <v>1949</v>
-      </c>
-      <c r="B71" s="4">
-        <v>13.89</v>
-      </c>
-      <c r="C71" s="6"/>
-      <c r="D71" s="6"/>
-      <c r="E71" s="6"/>
+        <v>1946</v>
+      </c>
+      <c r="B71" s="5">
+        <v>13.93</v>
+      </c>
+      <c r="D71" s="2"/>
+      <c r="E71" s="2"/>
     </row>
     <row r="72" spans="1:5">
       <c r="A72" s="3">
-        <v>1950</v>
-      </c>
-      <c r="B72" s="4">
-        <v>13.81</v>
-      </c>
-      <c r="C72" s="6"/>
-      <c r="D72" s="6"/>
-      <c r="E72" s="6"/>
+        <v>1947</v>
+      </c>
+      <c r="B72" s="5">
+        <v>13.96</v>
+      </c>
+      <c r="D72" s="2"/>
+      <c r="E72" s="2"/>
     </row>
     <row r="73" spans="1:5">
       <c r="A73" s="3">
-        <v>1951</v>
-      </c>
-      <c r="B73" s="4">
-        <v>13.94</v>
-      </c>
-      <c r="D73" s="6"/>
-      <c r="E73" s="6"/>
+        <v>1948</v>
+      </c>
+      <c r="B73" s="5">
+        <v>13.9</v>
+      </c>
+      <c r="D73" s="2"/>
+      <c r="E73" s="2"/>
     </row>
     <row r="74" spans="1:5">
       <c r="A74" s="3">
-        <v>1952</v>
-      </c>
-      <c r="B74" s="4">
-        <v>14.02</v>
-      </c>
-      <c r="D74" s="6"/>
-      <c r="E74" s="6"/>
+        <v>1949</v>
+      </c>
+      <c r="B74" s="5">
+        <v>13.89</v>
+      </c>
+      <c r="C74" s="11"/>
+      <c r="D74" s="2"/>
+      <c r="E74" s="2"/>
     </row>
     <row r="75" spans="1:5">
       <c r="A75" s="3">
-        <v>1953</v>
-      </c>
-      <c r="B75" s="4">
-        <v>14.09</v>
-      </c>
-      <c r="D75" s="6"/>
-      <c r="E75" s="6"/>
+        <v>1950</v>
+      </c>
+      <c r="B75" s="5">
+        <v>13.81</v>
+      </c>
+      <c r="C75" s="11"/>
+      <c r="D75" s="2"/>
+      <c r="E75" s="2"/>
     </row>
     <row r="76" spans="1:5">
       <c r="A76" s="3">
-        <v>1954</v>
-      </c>
-      <c r="B76" s="4">
-        <v>13.89</v>
-      </c>
-      <c r="D76" s="6"/>
-      <c r="E76" s="6"/>
+        <v>1951</v>
+      </c>
+      <c r="B76" s="5">
+        <v>13.94</v>
+      </c>
+      <c r="D76" s="2"/>
+      <c r="E76" s="2"/>
     </row>
     <row r="77" spans="1:5">
       <c r="A77" s="3">
-        <v>1955</v>
-      </c>
-      <c r="B77" s="4">
-        <v>13.88</v>
-      </c>
-      <c r="D77" s="6"/>
-      <c r="E77" s="6"/>
+        <v>1952</v>
+      </c>
+      <c r="B77" s="5">
+        <v>14.02</v>
+      </c>
+      <c r="D77" s="2"/>
+      <c r="E77" s="2"/>
     </row>
     <row r="78" spans="1:5">
       <c r="A78" s="3">
-        <v>1956</v>
-      </c>
-      <c r="B78" s="4">
-        <v>13.82</v>
-      </c>
-      <c r="D78" s="6"/>
-      <c r="E78" s="6"/>
+        <v>1953</v>
+      </c>
+      <c r="B78" s="5">
+        <v>14.09</v>
+      </c>
+      <c r="D78" s="2"/>
+      <c r="E78" s="2"/>
     </row>
     <row r="79" spans="1:5">
       <c r="A79" s="3">
-        <v>1957</v>
-      </c>
-      <c r="B79" s="4">
-        <v>14.03</v>
-      </c>
-      <c r="D79" s="6"/>
-      <c r="E79" s="6"/>
+        <v>1954</v>
+      </c>
+      <c r="B79" s="5">
+        <v>13.89</v>
+      </c>
+      <c r="D79" s="2"/>
+      <c r="E79" s="2"/>
     </row>
     <row r="80" spans="1:5">
       <c r="A80" s="3">
-        <v>1958</v>
-      </c>
-      <c r="B80" s="4">
-        <v>14.05</v>
-      </c>
-      <c r="D80" s="6"/>
-      <c r="E80" s="6"/>
+        <v>1955</v>
+      </c>
+      <c r="B80" s="5">
+        <v>13.88</v>
+      </c>
+      <c r="D80" s="2"/>
+      <c r="E80" s="2"/>
     </row>
     <row r="81" spans="1:5">
       <c r="A81" s="3">
-        <v>1959</v>
-      </c>
-      <c r="B81" s="4">
-        <v>14.03</v>
-      </c>
-      <c r="C81" s="6"/>
-      <c r="D81" s="6"/>
-      <c r="E81" s="6"/>
+        <v>1956</v>
+      </c>
+      <c r="B81" s="5">
+        <v>13.82</v>
+      </c>
+      <c r="D81" s="2"/>
+      <c r="E81" s="2"/>
     </row>
     <row r="82" spans="1:5">
       <c r="A82" s="3">
-        <v>1960</v>
-      </c>
-      <c r="B82" s="4">
-        <v>13.96</v>
-      </c>
-      <c r="C82" s="6"/>
-      <c r="D82" s="6"/>
-      <c r="E82" s="6"/>
+        <v>1957</v>
+      </c>
+      <c r="B82" s="5">
+        <v>14.03</v>
+      </c>
+      <c r="D82" s="2"/>
+      <c r="E82" s="2"/>
     </row>
     <row r="83" spans="1:5">
       <c r="A83" s="3">
-        <v>1961</v>
-      </c>
-      <c r="B83" s="4">
+        <v>1958</v>
+      </c>
+      <c r="B83" s="5">
         <v>14.05</v>
       </c>
-      <c r="D83" s="6"/>
-      <c r="E83" s="6"/>
+      <c r="D83" s="2"/>
+      <c r="E83" s="2"/>
     </row>
     <row r="84" spans="1:5">
       <c r="A84" s="3">
-        <v>1962</v>
-      </c>
-      <c r="B84" s="4">
-        <v>14.04</v>
-      </c>
-      <c r="D84" s="6"/>
-      <c r="E84" s="6"/>
+        <v>1959</v>
+      </c>
+      <c r="B84" s="5">
+        <v>14.03</v>
+      </c>
+      <c r="C84" s="11"/>
+      <c r="D84" s="2"/>
+      <c r="E84" s="2"/>
     </row>
     <row r="85" spans="1:5">
       <c r="A85" s="3">
-        <v>1963</v>
-      </c>
-      <c r="B85" s="4">
-        <v>14.08</v>
-      </c>
-      <c r="D85" s="6"/>
-      <c r="E85" s="6"/>
+        <v>1960</v>
+      </c>
+      <c r="B85" s="5">
+        <v>13.96</v>
+      </c>
+      <c r="C85" s="11"/>
+      <c r="D85" s="2"/>
+      <c r="E85" s="2"/>
     </row>
     <row r="86" spans="1:5">
       <c r="A86" s="3">
-        <v>1964</v>
-      </c>
-      <c r="B86" s="4">
-        <v>13.81</v>
-      </c>
-      <c r="D86" s="6"/>
-      <c r="E86" s="6"/>
+        <v>1961</v>
+      </c>
+      <c r="B86" s="5">
+        <v>14.05</v>
+      </c>
+      <c r="D86" s="2"/>
+      <c r="E86" s="2"/>
     </row>
     <row r="87" spans="1:5">
       <c r="A87" s="3">
-        <v>1965</v>
-      </c>
-      <c r="B87" s="4">
-        <v>13.9</v>
-      </c>
-      <c r="D87" s="6"/>
-      <c r="E87" s="6"/>
+        <v>1962</v>
+      </c>
+      <c r="B87" s="5">
+        <v>14.04</v>
+      </c>
+      <c r="D87" s="2"/>
+      <c r="E87" s="2"/>
     </row>
     <row r="88" spans="1:5">
       <c r="A88" s="3">
-        <v>1966</v>
-      </c>
-      <c r="B88" s="4">
-        <v>13.96</v>
-      </c>
-      <c r="D88" s="6"/>
-      <c r="E88" s="6"/>
+        <v>1963</v>
+      </c>
+      <c r="B88" s="5">
+        <v>14.08</v>
+      </c>
+      <c r="D88" s="2"/>
+      <c r="E88" s="2"/>
     </row>
     <row r="89" spans="1:5">
       <c r="A89" s="3">
-        <v>1967</v>
-      </c>
-      <c r="B89" s="4">
-        <v>13.99</v>
-      </c>
-      <c r="D89" s="6"/>
-      <c r="E89" s="6"/>
+        <v>1964</v>
+      </c>
+      <c r="B89" s="5">
+        <v>13.81</v>
+      </c>
+      <c r="D89" s="2"/>
+      <c r="E89" s="2"/>
     </row>
     <row r="90" spans="1:5">
       <c r="A90" s="3">
-        <v>1968</v>
-      </c>
-      <c r="B90" s="4">
-        <v>13.95</v>
-      </c>
-      <c r="C90" s="6"/>
-      <c r="D90" s="6"/>
-      <c r="E90" s="6"/>
+        <v>1965</v>
+      </c>
+      <c r="B90" s="5">
+        <v>13.9</v>
+      </c>
+      <c r="D90" s="2"/>
+      <c r="E90" s="2"/>
     </row>
     <row r="91" spans="1:5">
       <c r="A91" s="3">
-        <v>1969</v>
-      </c>
-      <c r="B91" s="4">
-        <v>14.06</v>
-      </c>
-      <c r="C91" s="6"/>
-      <c r="D91" s="6"/>
-      <c r="E91" s="6"/>
+        <v>1966</v>
+      </c>
+      <c r="B91" s="5">
+        <v>13.96</v>
+      </c>
+      <c r="D91" s="2"/>
+      <c r="E91" s="2"/>
     </row>
     <row r="92" spans="1:5">
       <c r="A92" s="3">
-        <v>1970</v>
-      </c>
-      <c r="B92" s="4">
-        <v>14.04</v>
-      </c>
-      <c r="C92" s="6"/>
-      <c r="D92" s="6"/>
-      <c r="E92" s="6"/>
+        <v>1967</v>
+      </c>
+      <c r="B92" s="5">
+        <v>13.99</v>
+      </c>
+      <c r="D92" s="2"/>
+      <c r="E92" s="2"/>
     </row>
     <row r="93" spans="1:5">
       <c r="A93" s="3">
-        <v>1971</v>
-      </c>
-      <c r="B93" s="4">
-        <v>13.93</v>
-      </c>
-      <c r="C93" s="6"/>
-      <c r="D93" s="6"/>
-      <c r="E93" s="6"/>
+        <v>1968</v>
+      </c>
+      <c r="B93" s="5">
+        <v>13.95</v>
+      </c>
+      <c r="C93" s="11"/>
+      <c r="D93" s="2"/>
+      <c r="E93" s="2"/>
     </row>
     <row r="94" spans="1:5">
       <c r="A94" s="3">
-        <v>1972</v>
-      </c>
-      <c r="B94" s="4">
-        <v>14.02</v>
-      </c>
-      <c r="C94" s="6"/>
-      <c r="D94" s="6"/>
-      <c r="E94" s="6"/>
+        <v>1969</v>
+      </c>
+      <c r="B94" s="5">
+        <v>14.06</v>
+      </c>
+      <c r="C94" s="11"/>
+      <c r="D94" s="2"/>
+      <c r="E94" s="2"/>
     </row>
     <row r="95" spans="1:5">
       <c r="A95" s="3">
-        <v>1973</v>
-      </c>
-      <c r="B95" s="4">
-        <v>14.15</v>
-      </c>
-      <c r="C95" s="6"/>
-      <c r="D95" s="6"/>
-      <c r="E95" s="6"/>
+        <v>1970</v>
+      </c>
+      <c r="B95" s="5">
+        <v>14.04</v>
+      </c>
+      <c r="C95" s="11"/>
+      <c r="D95" s="2"/>
+      <c r="E95" s="2"/>
     </row>
     <row r="96" spans="1:5">
       <c r="A96" s="3">
-        <v>1974</v>
-      </c>
-      <c r="B96" s="4">
+        <v>1971</v>
+      </c>
+      <c r="B96" s="5">
         <v>13.93</v>
       </c>
-      <c r="C96" s="6"/>
-      <c r="D96" s="6"/>
-      <c r="E96" s="6"/>
+      <c r="C96" s="11"/>
+      <c r="D96" s="2"/>
+      <c r="E96" s="2"/>
     </row>
     <row r="97" spans="1:5">
       <c r="A97" s="3">
-        <v>1975</v>
-      </c>
-      <c r="B97" s="4">
-        <v>13.99</v>
-      </c>
-      <c r="C97" s="6"/>
-      <c r="D97" s="6"/>
-      <c r="E97" s="6"/>
+        <v>1972</v>
+      </c>
+      <c r="B97" s="5">
+        <v>14.02</v>
+      </c>
+      <c r="C97" s="11"/>
+      <c r="D97" s="2"/>
+      <c r="E97" s="2"/>
     </row>
     <row r="98" spans="1:5">
       <c r="A98" s="3">
-        <v>1976</v>
-      </c>
-      <c r="B98" s="4">
-        <v>13.88</v>
-      </c>
-      <c r="C98" s="6"/>
-      <c r="D98" s="6"/>
-      <c r="E98" s="6"/>
+        <v>1973</v>
+      </c>
+      <c r="B98" s="5">
+        <v>14.15</v>
+      </c>
+      <c r="C98" s="11"/>
+      <c r="D98" s="2"/>
+      <c r="E98" s="2"/>
     </row>
     <row r="99" spans="1:5">
       <c r="A99" s="3">
-        <v>1977</v>
-      </c>
-      <c r="B99" s="4">
-        <v>14.14</v>
-      </c>
-      <c r="C99" s="6"/>
-      <c r="D99" s="6"/>
-      <c r="E99" s="6"/>
+        <v>1974</v>
+      </c>
+      <c r="B99" s="5">
+        <v>13.93</v>
+      </c>
+      <c r="C99" s="11"/>
+      <c r="D99" s="2"/>
+      <c r="E99" s="2"/>
     </row>
     <row r="100" spans="1:5">
       <c r="A100" s="3">
-        <v>1978</v>
-      </c>
-      <c r="B100" s="4">
-        <v>14.05</v>
-      </c>
-      <c r="C100" s="6"/>
-      <c r="D100" s="6"/>
-      <c r="E100" s="6"/>
+        <v>1975</v>
+      </c>
+      <c r="B100" s="5">
+        <v>13.99</v>
+      </c>
+      <c r="C100" s="11"/>
+      <c r="D100" s="2"/>
+      <c r="E100" s="2"/>
     </row>
     <row r="101" spans="1:5">
       <c r="A101" s="3">
-        <v>1979</v>
-      </c>
-      <c r="B101" s="4">
-        <v>14.11</v>
-      </c>
-      <c r="C101" s="6"/>
-      <c r="D101" s="6"/>
-      <c r="E101" s="6"/>
+        <v>1976</v>
+      </c>
+      <c r="B101" s="5">
+        <v>13.88</v>
+      </c>
+      <c r="C101" s="11"/>
+      <c r="D101" s="2"/>
+      <c r="E101" s="2"/>
     </row>
     <row r="102" spans="1:5">
       <c r="A102" s="3">
-        <v>1980</v>
-      </c>
-      <c r="B102" s="4">
-        <v>14.22</v>
-      </c>
-      <c r="C102" s="6"/>
-      <c r="D102" s="6"/>
-      <c r="E102" s="6"/>
+        <v>1977</v>
+      </c>
+      <c r="B102" s="5">
+        <v>14.14</v>
+      </c>
+      <c r="C102" s="11"/>
+      <c r="D102" s="2"/>
+      <c r="E102" s="2"/>
     </row>
     <row r="103" spans="1:5">
       <c r="A103" s="3">
-        <v>1981</v>
-      </c>
-      <c r="B103" s="4">
-        <v>14.28</v>
-      </c>
-      <c r="C103" s="6"/>
-      <c r="D103" s="6"/>
-      <c r="E103" s="6"/>
+        <v>1978</v>
+      </c>
+      <c r="B103" s="5">
+        <v>14.05</v>
+      </c>
+      <c r="C103" s="11"/>
+      <c r="D103" s="2"/>
+      <c r="E103" s="2"/>
     </row>
     <row r="104" spans="1:5">
       <c r="A104" s="3">
-        <v>1982</v>
-      </c>
-      <c r="B104" s="4">
-        <v>14.09</v>
-      </c>
-      <c r="C104" s="6"/>
-      <c r="D104" s="6"/>
-      <c r="E104" s="6"/>
+        <v>1979</v>
+      </c>
+      <c r="B104" s="5">
+        <v>14.11</v>
+      </c>
+      <c r="C104" s="11"/>
+      <c r="D104" s="2"/>
+      <c r="E104" s="2"/>
     </row>
     <row r="105" spans="1:5">
       <c r="A105" s="3">
-        <v>1983</v>
-      </c>
-      <c r="B105" s="4">
-        <v>14.27</v>
-      </c>
-      <c r="C105" s="6"/>
-      <c r="D105" s="6"/>
-      <c r="E105" s="6"/>
+        <v>1980</v>
+      </c>
+      <c r="B105" s="5">
+        <v>14.22</v>
+      </c>
+      <c r="C105" s="11"/>
+      <c r="D105" s="2"/>
+      <c r="E105" s="2"/>
     </row>
     <row r="106" spans="1:5">
       <c r="A106" s="3">
-        <v>1984</v>
-      </c>
-      <c r="B106" s="4">
-        <v>14.11</v>
-      </c>
-      <c r="C106" s="6"/>
-      <c r="D106" s="6"/>
-      <c r="E106" s="6"/>
+        <v>1981</v>
+      </c>
+      <c r="B106" s="5">
+        <v>14.28</v>
+      </c>
+      <c r="C106" s="11"/>
+      <c r="D106" s="2"/>
+      <c r="E106" s="2"/>
     </row>
     <row r="107" spans="1:5">
       <c r="A107" s="3">
-        <v>1985</v>
-      </c>
-      <c r="B107" s="4">
-        <v>14.08</v>
-      </c>
-      <c r="C107" s="6"/>
-      <c r="D107" s="6"/>
-      <c r="E107" s="6"/>
+        <v>1982</v>
+      </c>
+      <c r="B107" s="5">
+        <v>14.09</v>
+      </c>
+      <c r="C107" s="11"/>
+      <c r="D107" s="2"/>
+      <c r="E107" s="2"/>
     </row>
     <row r="108" spans="1:5">
       <c r="A108" s="3">
-        <v>1986</v>
-      </c>
-      <c r="B108" s="4">
-        <v>14.14</v>
-      </c>
-      <c r="C108" s="6"/>
-      <c r="D108" s="6"/>
-      <c r="E108" s="6"/>
+        <v>1983</v>
+      </c>
+      <c r="B108" s="5">
+        <v>14.27</v>
+      </c>
+      <c r="C108" s="11"/>
+      <c r="D108" s="2"/>
+      <c r="E108" s="2"/>
     </row>
     <row r="109" spans="1:5">
       <c r="A109" s="3">
-        <v>1987</v>
-      </c>
-      <c r="B109" s="4">
-        <v>14.28</v>
-      </c>
-      <c r="C109" s="6"/>
-      <c r="D109" s="6"/>
-      <c r="E109" s="6"/>
+        <v>1984</v>
+      </c>
+      <c r="B109" s="5">
+        <v>14.11</v>
+      </c>
+      <c r="C109" s="11"/>
+      <c r="D109" s="2"/>
+      <c r="E109" s="2"/>
     </row>
     <row r="110" spans="1:5">
       <c r="A110" s="3">
-        <v>1988</v>
-      </c>
-      <c r="B110" s="4">
-        <v>14.35</v>
-      </c>
-      <c r="C110" s="6"/>
-      <c r="D110" s="6"/>
-      <c r="E110" s="6"/>
+        <v>1985</v>
+      </c>
+      <c r="B110" s="5">
+        <v>14.08</v>
+      </c>
+      <c r="C110" s="11"/>
+      <c r="D110" s="2"/>
+      <c r="E110" s="2"/>
     </row>
     <row r="111" spans="1:5">
       <c r="A111" s="3">
-        <v>1989</v>
-      </c>
-      <c r="B111" s="4">
-        <v>14.24</v>
-      </c>
-      <c r="C111" s="6"/>
-      <c r="D111" s="6"/>
-      <c r="E111" s="6"/>
+        <v>1986</v>
+      </c>
+      <c r="B111" s="5">
+        <v>14.14</v>
+      </c>
+      <c r="C111" s="11"/>
+      <c r="D111" s="2"/>
+      <c r="E111" s="2"/>
     </row>
     <row r="112" spans="1:5">
       <c r="A112" s="3">
-        <v>1990</v>
-      </c>
-      <c r="B112" s="4">
-        <v>14.39</v>
-      </c>
-      <c r="C112" s="6"/>
-      <c r="D112" s="6"/>
-      <c r="E112" s="6"/>
+        <v>1987</v>
+      </c>
+      <c r="B112" s="5">
+        <v>14.28</v>
+      </c>
+      <c r="C112" s="11"/>
+      <c r="D112" s="2"/>
+      <c r="E112" s="2"/>
     </row>
     <row r="113" spans="1:5">
       <c r="A113" s="3">
-        <v>1991</v>
-      </c>
-      <c r="B113" s="4">
-        <v>14.38</v>
-      </c>
-      <c r="C113" s="6"/>
-      <c r="D113" s="6"/>
-      <c r="E113" s="6"/>
+        <v>1988</v>
+      </c>
+      <c r="B113" s="5">
+        <v>14.35</v>
+      </c>
+      <c r="C113" s="11"/>
+      <c r="D113" s="2"/>
+      <c r="E113" s="2"/>
     </row>
     <row r="114" spans="1:5">
       <c r="A114" s="3">
-        <v>1992</v>
-      </c>
-      <c r="B114" s="4">
-        <v>14.19</v>
-      </c>
-      <c r="C114" s="6"/>
-      <c r="D114" s="6"/>
-      <c r="E114" s="6"/>
+        <v>1989</v>
+      </c>
+      <c r="B114" s="5">
+        <v>14.24</v>
+      </c>
+      <c r="C114" s="11"/>
+      <c r="D114" s="2"/>
+      <c r="E114" s="2"/>
     </row>
     <row r="115" spans="1:5">
       <c r="A115" s="3">
-        <v>1993</v>
-      </c>
-      <c r="B115" s="4">
-        <v>14.2</v>
-      </c>
-      <c r="C115" s="6"/>
-      <c r="D115" s="6"/>
-      <c r="E115" s="6"/>
+        <v>1990</v>
+      </c>
+      <c r="B115" s="5">
+        <v>14.39</v>
+      </c>
+      <c r="C115" s="11"/>
+      <c r="D115" s="2"/>
+      <c r="E115" s="2"/>
     </row>
     <row r="116" spans="1:5">
       <c r="A116" s="3">
-        <v>1994</v>
-      </c>
-      <c r="B116" s="4">
-        <v>14.28</v>
-      </c>
-      <c r="C116" s="6"/>
-      <c r="D116" s="6"/>
-      <c r="E116" s="6"/>
+        <v>1991</v>
+      </c>
+      <c r="B116" s="5">
+        <v>14.38</v>
+      </c>
+      <c r="C116" s="11"/>
+      <c r="D116" s="2"/>
+      <c r="E116" s="2"/>
     </row>
     <row r="117" spans="1:5">
       <c r="A117" s="3">
-        <v>1995</v>
-      </c>
-      <c r="B117" s="4">
-        <v>14.42</v>
-      </c>
-      <c r="C117" s="6"/>
-      <c r="D117" s="6"/>
-      <c r="E117" s="6"/>
+        <v>1992</v>
+      </c>
+      <c r="B117" s="5">
+        <v>14.19</v>
+      </c>
+      <c r="C117" s="11"/>
+      <c r="D117" s="2"/>
+      <c r="E117" s="2"/>
     </row>
     <row r="118" spans="1:5">
       <c r="A118" s="3">
-        <v>1996</v>
-      </c>
-      <c r="B118" s="4">
-        <v>14.32</v>
-      </c>
-      <c r="C118" s="6"/>
-      <c r="D118" s="6"/>
-      <c r="E118" s="6"/>
+        <v>1993</v>
+      </c>
+      <c r="B118" s="5">
+        <v>14.2</v>
+      </c>
+      <c r="C118" s="11"/>
+      <c r="D118" s="2"/>
+      <c r="E118" s="2"/>
     </row>
     <row r="119" spans="1:5">
       <c r="A119" s="3">
-        <v>1997</v>
-      </c>
-      <c r="B119" s="4">
-        <v>14.45</v>
-      </c>
-      <c r="C119" s="6"/>
-      <c r="D119" s="6"/>
-      <c r="E119" s="6"/>
+        <v>1994</v>
+      </c>
+      <c r="B119" s="5">
+        <v>14.28</v>
+      </c>
+      <c r="C119" s="11"/>
+      <c r="D119" s="2"/>
+      <c r="E119" s="2"/>
     </row>
     <row r="120" spans="1:5">
       <c r="A120" s="3">
-        <v>1998</v>
-      </c>
-      <c r="B120" s="4">
-        <v>14.61</v>
-      </c>
-      <c r="C120" s="6"/>
-      <c r="D120" s="6"/>
-      <c r="E120" s="6"/>
+        <v>1995</v>
+      </c>
+      <c r="B120" s="5">
+        <v>14.42</v>
+      </c>
+      <c r="C120" s="11"/>
+      <c r="D120" s="2"/>
+      <c r="E120" s="2"/>
     </row>
     <row r="121" spans="1:5">
       <c r="A121" s="3">
-        <v>1999</v>
-      </c>
-      <c r="B121" s="4">
-        <v>14.39</v>
-      </c>
-      <c r="C121" s="6"/>
-      <c r="D121" s="6"/>
-      <c r="E121" s="6"/>
+        <v>1996</v>
+      </c>
+      <c r="B121" s="5">
+        <v>14.32</v>
+      </c>
+      <c r="C121" s="11"/>
+      <c r="D121" s="2"/>
+      <c r="E121" s="2"/>
     </row>
     <row r="122" spans="1:5">
       <c r="A122" s="3">
-        <v>2000</v>
-      </c>
-      <c r="B122" s="4">
-        <v>14.4</v>
-      </c>
-      <c r="C122" s="6"/>
-      <c r="D122" s="6"/>
-      <c r="E122" s="6"/>
+        <v>1997</v>
+      </c>
+      <c r="B122" s="5">
+        <v>14.45</v>
+      </c>
+      <c r="C122" s="11"/>
+      <c r="D122" s="2"/>
+      <c r="E122" s="2"/>
     </row>
     <row r="123" spans="1:5">
       <c r="A123" s="3">
-        <v>2001</v>
-      </c>
-      <c r="B123" s="4">
-        <v>14.52</v>
-      </c>
-      <c r="C123" s="6"/>
-      <c r="D123" s="6"/>
-      <c r="E123" s="6"/>
+        <v>1998</v>
+      </c>
+      <c r="B123" s="5">
+        <v>14.61</v>
+      </c>
+      <c r="C123" s="11"/>
+      <c r="D123" s="2"/>
+      <c r="E123" s="2"/>
     </row>
     <row r="124" spans="1:5">
       <c r="A124" s="3">
-        <v>2002</v>
-      </c>
-      <c r="B124" s="4">
-        <v>14.6</v>
-      </c>
-      <c r="C124" s="6"/>
-      <c r="D124" s="6"/>
-      <c r="E124" s="6"/>
+        <v>1999</v>
+      </c>
+      <c r="B124" s="5">
+        <v>14.39</v>
+      </c>
+      <c r="C124" s="11"/>
+      <c r="D124" s="2"/>
+      <c r="E124" s="2"/>
     </row>
     <row r="125" spans="1:5">
       <c r="A125" s="3">
-        <v>2003</v>
-      </c>
-      <c r="B125" s="4">
-        <v>14.59</v>
-      </c>
-      <c r="C125" s="6"/>
-      <c r="D125" s="6"/>
-      <c r="E125" s="6"/>
+        <v>2000</v>
+      </c>
+      <c r="B125" s="5">
+        <v>14.4</v>
+      </c>
+      <c r="C125" s="11"/>
+      <c r="D125" s="2"/>
+      <c r="E125" s="2"/>
     </row>
     <row r="126" spans="1:5">
       <c r="A126" s="3">
-        <v>2004</v>
-      </c>
-      <c r="B126" s="4">
-        <v>14.51</v>
-      </c>
-      <c r="C126" s="6"/>
-      <c r="D126" s="6"/>
-      <c r="E126" s="6"/>
+        <v>2001</v>
+      </c>
+      <c r="B126" s="5">
+        <v>14.52</v>
+      </c>
+      <c r="C126" s="11"/>
+      <c r="D126" s="2"/>
+      <c r="E126" s="2"/>
     </row>
     <row r="127" spans="1:5">
       <c r="A127" s="3">
-        <v>2005</v>
-      </c>
-      <c r="B127" s="4">
-        <v>14.65</v>
-      </c>
-      <c r="C127" s="6"/>
-      <c r="D127" s="6"/>
-      <c r="E127" s="6"/>
+        <v>2002</v>
+      </c>
+      <c r="B127" s="5">
+        <v>14.6</v>
+      </c>
+      <c r="C127" s="11"/>
+      <c r="D127" s="2"/>
+      <c r="E127" s="2"/>
     </row>
     <row r="128" spans="1:5">
       <c r="A128" s="3">
+        <v>2003</v>
+      </c>
+      <c r="B128" s="5">
+        <v>14.59</v>
+      </c>
+      <c r="C128" s="11"/>
+      <c r="D128" s="2"/>
+      <c r="E128" s="2"/>
+    </row>
+    <row r="129" spans="1:5">
+      <c r="A129" s="3">
+        <v>2004</v>
+      </c>
+      <c r="B129" s="5">
+        <v>14.51</v>
+      </c>
+      <c r="C129" s="11"/>
+      <c r="D129" s="2"/>
+      <c r="E129" s="2"/>
+    </row>
+    <row r="130" spans="1:5">
+      <c r="A130" s="3">
+        <v>2005</v>
+      </c>
+      <c r="B130" s="5">
+        <v>14.65</v>
+      </c>
+      <c r="C130" s="11"/>
+      <c r="D130" s="2"/>
+      <c r="E130" s="2"/>
+    </row>
+    <row r="131" spans="1:5">
+      <c r="A131" s="3">
         <v>2006</v>
       </c>
-      <c r="B128" s="4">
+      <c r="B131" s="5">
         <v>14.59</v>
       </c>
-      <c r="C128" s="6"/>
-      <c r="D128" s="6"/>
-      <c r="E128" s="6"/>
-    </row>
-    <row r="129" spans="1:5">
-      <c r="A129" s="8">
+      <c r="C131" s="11"/>
+      <c r="D131" s="2"/>
+      <c r="E131" s="2"/>
+    </row>
+    <row r="132" spans="1:5">
+      <c r="A132" s="3">
         <v>2007</v>
       </c>
-      <c r="B129" s="4">
+      <c r="B132" s="5">
         <v>14.62</v>
       </c>
-      <c r="C129" s="6"/>
-      <c r="D129" s="6"/>
-      <c r="E129" s="6"/>
-    </row>
-    <row r="130" spans="1:5">
-      <c r="A130" s="8">
+      <c r="C132" s="11"/>
+      <c r="D132" s="2"/>
+      <c r="E132" s="2"/>
+    </row>
+    <row r="133" spans="1:5">
+      <c r="A133" s="3">
         <v>2008</v>
       </c>
-      <c r="B130" s="4">
+      <c r="B133" s="5">
         <v>14.49</v>
       </c>
-      <c r="C130" s="6"/>
-      <c r="D130" s="6"/>
-      <c r="E130" s="6"/>
-    </row>
-    <row r="131" spans="1:5">
-      <c r="A131" s="8">
+      <c r="C133" s="11"/>
+      <c r="D133" s="2"/>
+      <c r="E133" s="2"/>
+    </row>
+    <row r="134" spans="1:5">
+      <c r="A134" s="3">
         <v>2009</v>
       </c>
-      <c r="B131" s="4">
+      <c r="B134" s="5">
         <v>14.59</v>
       </c>
-      <c r="C131" s="6"/>
-      <c r="D131" s="6"/>
-      <c r="E131" s="6"/>
-    </row>
-    <row r="132" spans="1:5">
-      <c r="A132" s="9">
+      <c r="C134" s="11"/>
+      <c r="D134" s="2"/>
+      <c r="E134" s="2"/>
+    </row>
+    <row r="135" spans="1:5">
+      <c r="A135" s="4">
         <v>2010</v>
       </c>
-      <c r="B132" s="10">
+      <c r="B135" s="5">
         <v>14.66</v>
       </c>
-      <c r="C132" s="6"/>
-      <c r="D132" s="6"/>
-      <c r="E132" s="6"/>
-    </row>
-    <row r="133" spans="1:5">
-      <c r="A133" s="9">
+      <c r="C135" s="11"/>
+      <c r="D135" s="2"/>
+      <c r="E135" s="2"/>
+    </row>
+    <row r="136" spans="1:5">
+      <c r="A136" s="4">
         <v>2011</v>
       </c>
-      <c r="B133" s="10">
+      <c r="B136" s="5">
         <v>14.55</v>
       </c>
-      <c r="C133" s="6"/>
-      <c r="D133" s="6"/>
-      <c r="E133" s="6"/>
-    </row>
-    <row r="134" spans="1:5">
-      <c r="A134" s="9">
+      <c r="C136" s="11"/>
+      <c r="D136" s="2"/>
+      <c r="E136" s="2"/>
+    </row>
+    <row r="137" spans="1:5">
+      <c r="A137" s="4">
         <v>2012</v>
       </c>
-      <c r="B134" s="10">
+      <c r="B137" s="5">
         <v>14.57</v>
       </c>
-      <c r="C134" s="6"/>
-      <c r="D134" s="6"/>
-      <c r="E134" s="6"/>
-    </row>
-    <row r="135" spans="1:5">
-      <c r="A135" s="8">
+      <c r="C137" s="11"/>
+      <c r="D137" s="2"/>
+      <c r="E137" s="2"/>
+    </row>
+    <row r="138" spans="1:5">
+      <c r="A138" s="3">
         <v>2013</v>
       </c>
-      <c r="B135" s="10">
+      <c r="B138" s="5">
         <v>14.6</v>
       </c>
-      <c r="C135" s="6"/>
-      <c r="D135" s="6"/>
-      <c r="E135" s="6"/>
-    </row>
-    <row r="136" spans="1:5">
-      <c r="A136" s="11">
+      <c r="C138" s="11"/>
+      <c r="D138" s="2"/>
+      <c r="E138" s="2"/>
+    </row>
+    <row r="139" spans="1:5">
+      <c r="A139" s="4">
         <v>2014</v>
       </c>
-      <c r="B136" s="12">
+      <c r="B139" s="5">
         <v>14.68</v>
       </c>
-      <c r="C136" s="6"/>
-      <c r="D136" s="6"/>
-      <c r="E136" s="6"/>
-    </row>
-    <row r="137" spans="1:5">
-      <c r="A137" s="8">
+      <c r="C139" s="11"/>
+      <c r="D139" s="2"/>
+      <c r="E139" s="2"/>
+    </row>
+    <row r="140" spans="1:5">
+      <c r="A140" s="3">
         <v>2015</v>
       </c>
-      <c r="B137" s="13">
+      <c r="B140" s="6">
         <v>14.87</v>
       </c>
     </row>
-    <row r="138" spans="1:5">
-      <c r="A138" s="11">
+    <row r="141" spans="1:5">
+      <c r="A141" s="4">
         <v>2016</v>
       </c>
-      <c r="B138" s="13">
+      <c r="B141" s="6">
         <v>14.99</v>
       </c>
     </row>
-    <row r="139" spans="1:5">
-      <c r="A139" s="8">
+    <row r="142" spans="1:5">
+      <c r="A142" s="3">
         <v>2017</v>
       </c>
-      <c r="B139" s="13">
+      <c r="B142" s="6">
         <v>14.9</v>
       </c>
     </row>
-    <row r="140" spans="1:5">
-      <c r="A140" s="11">
+    <row r="143" spans="1:5">
+      <c r="A143" s="4">
         <v>2018</v>
       </c>
-      <c r="B140" s="13">
+      <c r="B143" s="6">
         <v>14.83</v>
       </c>
     </row>

</xml_diff>